<commit_message>
calculate Square & refactoring
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="12525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
   <si>
     <t>P</t>
   </si>
@@ -38,15 +38,45 @@
   <si>
     <t>p</t>
   </si>
+  <si>
+    <t>Треугольники, расчет по формуле</t>
+  </si>
+  <si>
+    <t>Пареллелограмм, расчет по формуле</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Отрезок 1</t>
+  </si>
+  <si>
+    <t>Отрезок 2</t>
+  </si>
+  <si>
+    <t>x1y1-x2y2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -100,11 +130,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -992,10 +1028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B4:X37"/>
+  <dimension ref="B2:AI37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA17" sqref="AA17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="AC30" sqref="AC30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1003,7 +1039,12 @@
     <col min="3" max="27" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:24">
+    <row r="2" spans="2:35">
+      <c r="W2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:35">
       <c r="B4">
         <v>15</v>
       </c>
@@ -1023,7 +1064,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="2:24">
+    <row r="5" spans="2:35">
       <c r="B5">
         <v>14</v>
       </c>
@@ -1055,7 +1096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:24">
+    <row r="6" spans="2:35">
       <c r="B6">
         <v>13</v>
       </c>
@@ -1083,8 +1124,36 @@
       <c r="X6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="2:24">
+      <c r="AB6" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="AC6" s="4">
+        <f>W6-W8</f>
+        <v>-6</v>
+      </c>
+      <c r="AD6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE6" s="4">
+        <f>X7-X8</f>
+        <v>5</v>
+      </c>
+      <c r="AF6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG6" s="4">
+        <f>W7-W8</f>
+        <v>-6</v>
+      </c>
+      <c r="AH6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AI6" s="4">
+        <f>X6-X8</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:35">
       <c r="B7">
         <v>12</v>
       </c>
@@ -1112,8 +1181,14 @@
       <c r="X7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="2:24">
+      <c r="AD7">
+        <v>-30</v>
+      </c>
+      <c r="AH7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:35">
       <c r="B8">
         <v>11</v>
       </c>
@@ -1141,8 +1216,20 @@
       <c r="X8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="2:24">
+      <c r="AB8">
+        <v>0.5</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE8">
+        <v>42</v>
+      </c>
+      <c r="AG8" s="5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:35">
       <c r="B9">
         <v>10</v>
       </c>
@@ -1162,7 +1249,7 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="2:24">
+    <row r="10" spans="2:35">
       <c r="B10">
         <v>9</v>
       </c>
@@ -1193,8 +1280,36 @@
       <c r="X10">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="2:24">
+      <c r="AB10">
+        <v>0.5</v>
+      </c>
+      <c r="AC10">
+        <f>W10-W12</f>
+        <v>-10</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE10">
+        <f>X11-X12</f>
+        <v>6</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG10">
+        <f>W11-W12</f>
+        <v>-5</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>9</v>
+      </c>
+      <c r="AI10">
+        <f>X10-X12</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:35">
       <c r="B11">
         <v>8</v>
       </c>
@@ -1222,8 +1337,14 @@
       <c r="X11">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="2:24">
+      <c r="AD11">
+        <v>-60</v>
+      </c>
+      <c r="AH11">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="12" spans="2:35">
       <c r="B12">
         <v>7</v>
       </c>
@@ -1251,8 +1372,20 @@
       <c r="X12">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="2:24">
+      <c r="AB12">
+        <v>0.5</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD12">
+        <v>30</v>
+      </c>
+      <c r="AG12" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:35">
       <c r="B13">
         <v>6</v>
       </c>
@@ -1272,7 +1405,7 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="2:24">
+    <row r="14" spans="2:35">
       <c r="B14">
         <v>5</v>
       </c>
@@ -1292,7 +1425,7 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="2:24">
+    <row r="15" spans="2:35">
       <c r="B15">
         <v>4</v>
       </c>
@@ -1312,7 +1445,7 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
-    <row r="16" spans="2:24">
+    <row r="16" spans="2:35">
       <c r="B16">
         <v>3</v>
       </c>
@@ -1332,7 +1465,7 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="2:24">
+    <row r="17" spans="2:29">
       <c r="B17">
         <v>2</v>
       </c>
@@ -1352,7 +1485,7 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="2:24">
+    <row r="18" spans="2:29">
       <c r="B18">
         <v>1</v>
       </c>
@@ -1372,7 +1505,7 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="2:24">
+    <row r="19" spans="2:29">
       <c r="B19">
         <v>0</v>
       </c>
@@ -1422,7 +1555,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="2:24">
+    <row r="20" spans="2:29">
+      <c r="V20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:29">
       <c r="B22">
         <v>15</v>
       </c>
@@ -1445,7 +1583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:24">
+    <row r="23" spans="2:29">
       <c r="B23">
         <v>14</v>
       </c>
@@ -1474,7 +1612,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:24">
+    <row r="24" spans="2:29">
       <c r="B24">
         <v>13</v>
       </c>
@@ -1503,7 +1641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="2:24">
+    <row r="25" spans="2:29">
       <c r="B25">
         <v>12</v>
       </c>
@@ -1532,7 +1670,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:24">
+    <row r="26" spans="2:29">
       <c r="B26">
         <v>11</v>
       </c>
@@ -1561,7 +1699,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="2:24">
+    <row r="27" spans="2:29">
       <c r="B27">
         <v>10</v>
       </c>
@@ -1581,7 +1719,7 @@
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
     </row>
-    <row r="28" spans="2:24">
+    <row r="28" spans="2:29">
       <c r="B28">
         <v>9</v>
       </c>
@@ -1612,8 +1750,14 @@
       <c r="X28">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="2:24">
+      <c r="AB28" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="2:29">
       <c r="B29">
         <v>8</v>
       </c>
@@ -1642,7 +1786,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="2:24">
+    <row r="30" spans="2:29">
       <c r="B30">
         <v>7</v>
       </c>
@@ -1670,8 +1814,11 @@
       <c r="X30">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="2:24">
+      <c r="AB30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="2:29">
       <c r="B31">
         <v>6</v>
       </c>
@@ -1691,7 +1838,7 @@
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
     </row>
-    <row r="32" spans="2:24">
+    <row r="32" spans="2:29">
       <c r="B32">
         <v>5</v>
       </c>
@@ -1843,7 +1990,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>